<commit_message>
eq workplan + monte carlo first wall diagram update
</commit_message>
<xml_diff>
--- a/nova/projects/equilibrium/work_plan.xlsx
+++ b/nova/projects/equilibrium/work_plan.xlsx
@@ -1200,9 +1200,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J137"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B77" sqref="B77"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1310,7 +1310,7 @@
         <v>16</v>
       </c>
       <c r="G5" s="3">
-        <v>46023</v>
+        <v>47088</v>
       </c>
       <c r="I5" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
SOFT updates biot cylinder dev
</commit_message>
<xml_diff>
--- a/nova/projects/equilibrium/work_plan.xlsx
+++ b/nova/projects/equilibrium/work_plan.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="482" uniqueCount="290">
   <si>
     <t>task</t>
   </si>
@@ -65,9 +65,6 @@
     <t>non-linear reconstruction</t>
   </si>
   <si>
-    <t>FP</t>
-  </si>
-  <si>
     <t>phase</t>
   </si>
   <si>
@@ -227,15 +224,9 @@
     <t>ms-mag-only</t>
   </si>
   <si>
-    <t>wm-disrupt-low</t>
-  </si>
-  <si>
     <t>wm-shield</t>
   </si>
   <si>
-    <t>wm-disrupt-half</t>
-  </si>
-  <si>
     <t>wm-shield-3d</t>
   </si>
   <si>
@@ -335,12 +326,6 @@
     <t>nlr-refactor</t>
   </si>
   <si>
-    <t>tune model to fit disruption behaviour (low current)</t>
-  </si>
-  <si>
-    <t>tune model to fit disruption behaviour (half current)</t>
-  </si>
-  <si>
     <t>baseline low-n stability metrics available</t>
   </si>
   <si>
@@ -530,9 +515,6 @@
     <t>lin-strain-nova</t>
   </si>
   <si>
-    <t>ms-lin-strain-nova</t>
-  </si>
-  <si>
     <t>ms-nova-trans</t>
   </si>
   <si>
@@ -545,18 +527,12 @@
     <t>in-house free-boundary equilibrium solver available</t>
   </si>
   <si>
-    <t>tune 2D wall model using 3D disruption simulations (Maxwell / Ansys)</t>
-  </si>
-  <si>
     <t>transient in-house free-boundary equilibrium solver available</t>
   </si>
   <si>
     <t>3D in-house free-boundary equilibrium solver available</t>
   </si>
   <si>
-    <t xml:space="preserve">separation of plasma and vessel current in advance of kinetic measurements </t>
-  </si>
-  <si>
     <t>magnetics-only diagnostics available</t>
   </si>
   <si>
@@ -569,9 +545,6 @@
     <t xml:space="preserve">tune TBM geometry from field measurements </t>
   </si>
   <si>
-    <t>measure open-loop vessel response (TF, PF, CS, VS3)</t>
-  </si>
-  <si>
     <t>PF-map3d</t>
   </si>
   <si>
@@ -632,9 +605,6 @@
     <t>lr-nova-pfpo1</t>
   </si>
   <si>
-    <t>develop non-linear parametrizations (flux functions - include rotation)</t>
-  </si>
-  <si>
     <t>refactor non-linear search for low-latency regression (ML model)</t>
   </si>
   <si>
@@ -776,9 +746,6 @@
     <t xml:space="preserve">develop 3D commissioning waveforms </t>
   </si>
   <si>
-    <t>build 3D ELM coil field maps + check transient response</t>
-  </si>
-  <si>
     <t>develop fast coupled VV-ELM coil transfer functions</t>
   </si>
   <si>
@@ -842,12 +809,6 @@
     <t>pekm-3d-pfpo1</t>
   </si>
   <si>
-    <t>fm-bay,sta-automatic,FP</t>
-  </si>
-  <si>
-    <t>tune 3D field maps from vacuum field measurements</t>
-  </si>
-  <si>
     <t>tune 3D ELM coil field maps from vacuum field measurements</t>
   </si>
   <si>
@@ -891,6 +852,48 @@
   </si>
   <si>
     <t>Kalman filter data assimilation available (synthetic analysis pipeline)</t>
+  </si>
+  <si>
+    <t>FP+EO</t>
+  </si>
+  <si>
+    <t>tune model to fit CS ramp</t>
+  </si>
+  <si>
+    <t>measure open-loop vessel response (PF, CS)</t>
+  </si>
+  <si>
+    <t>wm-CS-ramp</t>
+  </si>
+  <si>
+    <t>build 3D ELM coil field maps + check predictions for transient response</t>
+  </si>
+  <si>
+    <t>tune 3D field maps from CC vacuum field measurements</t>
+  </si>
+  <si>
+    <t>nl-pfpo1-support</t>
+  </si>
+  <si>
+    <t>nl-pfpo3-support</t>
+  </si>
+  <si>
+    <t>tune 2D wall model using 3D vessel CS ramp and disruption simulations</t>
+  </si>
+  <si>
+    <t>test eddy current and power supply models</t>
+  </si>
+  <si>
+    <t>test-nova-eddy</t>
+  </si>
+  <si>
+    <t>develop non-linear parametrizations (extend flux functions - include rotation &amp; fast ions)</t>
+  </si>
+  <si>
+    <t>apply causal reconstruction workflow in support of PFPO-2</t>
+  </si>
+  <si>
+    <t>pekm-3d-pfpo2</t>
   </si>
 </sst>
 </file>
@@ -1229,11 +1232,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K152"/>
+  <dimension ref="A1:K154"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A88" sqref="A88"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A125" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D138" sqref="D138"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1258,7 +1261,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>4</v>
@@ -1267,10 +1270,10 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>6</v>
@@ -1279,29 +1282,29 @@
         <v>7</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D2">
         <f>4*12+3</f>
         <v>51</v>
       </c>
       <c r="E2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="1"/>
@@ -1311,19 +1314,19 @@
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D3">
         <v>14</v>
       </c>
       <c r="E3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="1"/>
@@ -1333,16 +1336,16 @@
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="2"/>
@@ -1355,20 +1358,20 @@
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B5" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D5">
         <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="2" t="s">
-        <v>13</v>
+        <v>276</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -1377,20 +1380,20 @@
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="F6" s="1"/>
       <c r="G6" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
@@ -1399,20 +1402,20 @@
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7">
         <v>18</v>
       </c>
       <c r="E7" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F7" s="1"/>
       <c r="G7" s="2" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" s="1"/>
@@ -1421,20 +1424,20 @@
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D8">
         <v>15</v>
       </c>
       <c r="E8" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F8" s="1"/>
       <c r="G8" s="2" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
@@ -1443,20 +1446,20 @@
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D9">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="F9" s="1"/>
       <c r="G9" s="2" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
@@ -1465,20 +1468,20 @@
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D10">
         <v>21</v>
       </c>
       <c r="E10" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
@@ -1487,20 +1490,20 @@
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D11">
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
@@ -1509,20 +1512,20 @@
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B12" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D12">
         <v>8</v>
       </c>
       <c r="E12" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="F12" s="1"/>
       <c r="G12" s="2" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
@@ -1531,20 +1534,20 @@
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D13">
         <v>16</v>
       </c>
       <c r="E13" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="2" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1553,20 +1556,20 @@
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D14">
         <v>8</v>
       </c>
       <c r="E14" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="2" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
@@ -1575,20 +1578,20 @@
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15">
         <v>16</v>
       </c>
       <c r="E15" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="2" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
@@ -1597,20 +1600,20 @@
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D16">
         <v>8</v>
       </c>
       <c r="E16" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
@@ -1619,20 +1622,20 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D17">
         <v>16</v>
       </c>
       <c r="E17" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
@@ -1641,20 +1644,20 @@
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D18">
         <v>9</v>
       </c>
       <c r="E18" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="2" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
@@ -1663,20 +1666,20 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D19">
         <v>16</v>
       </c>
       <c r="E19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="2" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
@@ -1685,20 +1688,20 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D20">
         <v>8</v>
       </c>
       <c r="E20" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="2" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
@@ -1707,20 +1710,20 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D21">
         <v>16</v>
       </c>
       <c r="E21" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="2" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
@@ -1729,20 +1732,20 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B22" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D22">
         <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="2" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
@@ -1751,20 +1754,20 @@
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B23" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D23">
         <v>16</v>
       </c>
       <c r="E23" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="2" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
@@ -1773,65 +1776,65 @@
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B25" t="s">
         <v>0</v>
       </c>
       <c r="C25" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="E25" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D26" s="5">
         <v>6</v>
       </c>
       <c r="E26" s="2" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="F26" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D27" s="5">
         <v>6</v>
       </c>
       <c r="E27" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="F27" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A28" s="2"/>
       <c r="B28" s="2" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" s="6">
         <v>0</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G28" s="2"/>
       <c r="H28" s="2"/>
@@ -1841,77 +1844,77 @@
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="D29" s="5">
         <v>3</v>
       </c>
       <c r="E29" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="G29" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D30" s="5">
         <v>0</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D31" s="5">
         <v>12</v>
       </c>
       <c r="E31" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D32" s="5">
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="G32" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="D33" s="5">
         <v>0</v>
       </c>
       <c r="E33" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G33" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.35">
@@ -1923,7 +1926,7 @@
       </c>
       <c r="D35" s="6"/>
       <c r="E35" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F35" s="2"/>
       <c r="G35" s="2"/>
@@ -1933,17 +1936,17 @@
     <row r="36" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A36" s="2"/>
       <c r="B36" s="2" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" s="6">
         <v>0</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="G36" s="2"/>
       <c r="H36" s="2"/>
@@ -1954,18 +1957,18 @@
     <row r="37" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A37" s="2"/>
       <c r="B37" s="2" t="s">
-        <v>275</v>
+        <v>262</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" s="6">
         <v>6</v>
       </c>
       <c r="E37" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="F37" s="2"/>
       <c r="G37" s="2" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
@@ -1975,18 +1978,18 @@
     <row r="38" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A38" s="2"/>
       <c r="B38" s="2" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" s="6">
         <v>3</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="F38" s="2"/>
       <c r="G38" s="2" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
@@ -1996,18 +1999,18 @@
     <row r="39" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A39" s="2"/>
       <c r="B39" s="2" t="s">
-        <v>209</v>
+        <v>199</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" s="6">
         <v>3</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="F39" s="2"/>
       <c r="G39" s="2" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="H39" s="2"/>
       <c r="I39" s="2"/>
@@ -2017,18 +2020,18 @@
     <row r="40" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A40" s="2"/>
       <c r="B40" s="2" t="s">
-        <v>276</v>
+        <v>263</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" s="6">
         <v>0</v>
       </c>
       <c r="E40" s="2" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="F40" s="2"/>
       <c r="G40" s="2" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="H40" s="2"/>
       <c r="I40" s="2"/>
@@ -2037,464 +2040,454 @@
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="D41" s="6">
         <v>3</v>
       </c>
       <c r="E41" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F41" s="2"/>
       <c r="G41" s="2" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="H41" s="7"/>
       <c r="I41" s="2"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D42" s="6">
         <v>6</v>
       </c>
       <c r="E42" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F42" s="2"/>
       <c r="G42" s="2" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="H42" s="2"/>
       <c r="I42" s="2"/>
       <c r="J42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
-        <v>204</v>
+        <v>194</v>
       </c>
       <c r="D43" s="6">
         <v>0</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F43" s="2"/>
       <c r="G43" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H43" s="2"/>
       <c r="I43" s="2"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="D44" s="6">
         <v>6</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="F44" s="2"/>
       <c r="G44" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="H44" s="2"/>
       <c r="I44" s="2"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
-        <v>277</v>
+        <v>264</v>
       </c>
       <c r="D45" s="6">
         <v>3</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F45" s="2"/>
       <c r="G45" s="2" t="s">
-        <v>206</v>
+        <v>196</v>
       </c>
       <c r="H45" s="2"/>
       <c r="I45" s="2"/>
     </row>
     <row r="46" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
-        <v>219</v>
+        <v>209</v>
       </c>
       <c r="D46" s="6">
         <v>6</v>
       </c>
       <c r="E46" s="2" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="F46" s="2"/>
       <c r="G46" s="2" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="H46" s="2"/>
       <c r="I46" s="2"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B47" t="s">
-        <v>176</v>
-      </c>
+      <c r="B47" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="C47" s="2"/>
       <c r="D47" s="6">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E47" s="2" t="s">
-        <v>168</v>
+        <v>192</v>
       </c>
       <c r="F47" s="2"/>
       <c r="G47" s="2" t="s">
-        <v>167</v>
+        <v>198</v>
       </c>
       <c r="H47" s="2"/>
       <c r="I47" s="2"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
-        <v>278</v>
+        <v>201</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F48" s="2"/>
       <c r="G48" s="2" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="H48" s="2"/>
       <c r="I48" s="2"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B49" s="2" t="s">
-        <v>211</v>
-      </c>
-      <c r="C49" s="2"/>
+      <c r="B49" t="s">
+        <v>160</v>
+      </c>
       <c r="D49" s="6">
         <v>3</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>210</v>
+        <v>91</v>
       </c>
       <c r="F49" s="2"/>
       <c r="G49" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
-        <v>165</v>
-      </c>
-      <c r="D50" s="6">
-        <v>3</v>
+        <v>202</v>
+      </c>
+      <c r="D50" s="5">
+        <v>6</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="F50" s="2"/>
+        <v>282</v>
+      </c>
       <c r="G50" s="2" t="s">
-        <v>210</v>
-      </c>
-      <c r="H50" s="2"/>
-      <c r="I50" s="2"/>
+        <v>221</v>
+      </c>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
-        <v>15</v>
-      </c>
-      <c r="B51" s="2"/>
-      <c r="C51" s="2"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="2"/>
-      <c r="F51" s="2"/>
-      <c r="G51" s="2"/>
-      <c r="H51" s="2"/>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
-      <c r="K51" s="2"/>
+      <c r="B51" t="s">
+        <v>226</v>
+      </c>
+      <c r="D51" s="5">
+        <v>6</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="6"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+      <c r="G52" s="2"/>
+      <c r="H52" s="2"/>
+      <c r="I52" s="2"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="2"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
         <v>12</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>0</v>
       </c>
-      <c r="E52" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B53" t="s">
-        <v>48</v>
-      </c>
-      <c r="D53" s="5">
-        <v>3</v>
-      </c>
       <c r="E53" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="G53" s="2" t="s">
-        <v>200</v>
+        <v>39</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
-        <v>202</v>
+        <v>47</v>
       </c>
       <c r="D54" s="5">
         <v>3</v>
       </c>
       <c r="E54" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G54" s="2" t="s">
-        <v>41</v>
+        <v>191</v>
       </c>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
-        <v>203</v>
+        <v>287</v>
       </c>
       <c r="D55" s="5">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E55" s="2" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
       <c r="G55" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
-        <v>107</v>
+        <v>193</v>
       </c>
       <c r="D56" s="5">
         <v>6</v>
       </c>
       <c r="E56" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="G56" s="2" t="s">
-        <v>102</v>
+        <v>41</v>
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
-        <v>207</v>
+        <v>102</v>
       </c>
       <c r="D57" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E57" s="2" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
       <c r="G57" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
-        <v>108</v>
+        <v>197</v>
       </c>
       <c r="D58" s="5">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E58" s="2" t="s">
-        <v>93</v>
+        <v>43</v>
       </c>
       <c r="G58" s="2" t="s">
-        <v>44</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
-        <v>212</v>
+        <v>103</v>
       </c>
       <c r="D59" s="5">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="E59" s="2" t="s">
-        <v>213</v>
+        <v>90</v>
       </c>
       <c r="G59" s="2" t="s">
-        <v>231</v>
+        <v>43</v>
       </c>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
-        <v>279</v>
+        <v>202</v>
       </c>
       <c r="D60" s="5">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E60" s="2" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>213</v>
+        <v>282</v>
       </c>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="C61" s="2"/>
-      <c r="D61" s="6">
-        <v>0</v>
+      <c r="B61" t="s">
+        <v>266</v>
+      </c>
+      <c r="D61" s="5">
+        <v>3</v>
       </c>
       <c r="E61" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="F61" s="2" t="s">
-        <v>128</v>
-      </c>
-      <c r="G61" s="2"/>
-      <c r="H61" s="2"/>
-      <c r="I61" s="2"/>
-      <c r="J61" s="2"/>
-      <c r="K61" s="2"/>
+        <v>204</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>203</v>
+      </c>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A62" s="2"/>
       <c r="B62" s="2" t="s">
-        <v>280</v>
+        <v>181</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E62" s="2" t="s">
-        <v>217</v>
-      </c>
-      <c r="F62" s="2"/>
-      <c r="G62" s="2" t="s">
-        <v>215</v>
-      </c>
+        <v>180</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="G62" s="2"/>
       <c r="H62" s="2"/>
       <c r="I62" s="2"/>
+      <c r="J62" s="2"/>
+      <c r="K62" s="2"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B63" s="2" t="s">
-        <v>216</v>
+        <v>267</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="F63" s="2"/>
       <c r="G63" s="2" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="H63" s="2"/>
       <c r="I63" s="2"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B64" t="s">
-        <v>166</v>
-      </c>
+      <c r="B64" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C64" s="2"/>
       <c r="D64" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E64" s="2" t="s">
-        <v>38</v>
+        <v>208</v>
       </c>
       <c r="F64" s="2"/>
       <c r="G64" s="2" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="H64" s="2"/>
       <c r="I64" s="2"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
-        <v>236</v>
-      </c>
-      <c r="D65" s="5">
-        <v>15</v>
+        <v>161</v>
+      </c>
+      <c r="D65" s="6">
+        <v>6</v>
       </c>
       <c r="E65" s="2" t="s">
-        <v>237</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="F65" s="2"/>
       <c r="G65" s="2" t="s">
-        <v>235</v>
-      </c>
+        <v>208</v>
+      </c>
+      <c r="H65" s="2"/>
+      <c r="I65" s="2"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A66" t="s">
-        <v>15</v>
-      </c>
-      <c r="E66" s="2"/>
-      <c r="G66" s="2"/>
+      <c r="B66" t="s">
+        <v>226</v>
+      </c>
+      <c r="D66" s="5">
+        <v>9</v>
+      </c>
+      <c r="E66" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="G66" s="2" t="s">
+        <v>283</v>
+      </c>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A67" t="s">
-        <v>221</v>
-      </c>
-      <c r="B67" t="s">
+        <v>14</v>
+      </c>
+      <c r="E67" s="2"/>
+      <c r="G67" s="2"/>
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A68" t="s">
+        <v>211</v>
+      </c>
+      <c r="B68" t="s">
         <v>0</v>
       </c>
-      <c r="D67" s="6"/>
-      <c r="E67" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="F67" s="2"/>
-      <c r="G67" s="2"/>
-      <c r="H67" s="2"/>
-      <c r="I67" s="2"/>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A68" s="2"/>
-      <c r="B68" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="C68" s="2"/>
-      <c r="D68" s="6">
-        <v>0</v>
-      </c>
+      <c r="D68" s="6"/>
       <c r="E68" s="2" t="s">
-        <v>66</v>
+        <v>213</v>
       </c>
       <c r="F68" s="2"/>
-      <c r="G68" s="2" t="s">
-        <v>123</v>
-      </c>
+      <c r="G68" s="2"/>
       <c r="H68" s="2"/>
       <c r="I68" s="2"/>
-      <c r="J68" s="2"/>
-      <c r="K68" s="2"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A69" s="2"/>
       <c r="B69" s="2" t="s">
-        <v>225</v>
+        <v>169</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E69" s="2" t="s">
-        <v>228</v>
+        <v>65</v>
       </c>
       <c r="F69" s="2"/>
       <c r="G69" s="2" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="H69" s="2"/>
       <c r="I69" s="2"/>
@@ -2504,18 +2497,18 @@
     <row r="70" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A70" s="2"/>
       <c r="B70" s="2" t="s">
-        <v>281</v>
+        <v>215</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" s="6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E70" s="2" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="F70" s="2"/>
       <c r="G70" s="2" t="s">
-        <v>228</v>
+        <v>118</v>
       </c>
       <c r="H70" s="2"/>
       <c r="I70" s="2"/>
@@ -2523,83 +2516,84 @@
       <c r="K70" s="2"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A71" s="2"/>
       <c r="B71" s="2" t="s">
-        <v>282</v>
+        <v>268</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" s="6">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="E71" s="2" t="s">
-        <v>226</v>
+        <v>219</v>
       </c>
       <c r="F71" s="2"/>
       <c r="G71" s="2" t="s">
-        <v>229</v>
+        <v>218</v>
       </c>
       <c r="H71" s="2"/>
       <c r="I71" s="2"/>
-      <c r="J71" t="s">
-        <v>17</v>
-      </c>
+      <c r="J71" s="2"/>
       <c r="K71" s="2"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B72" s="2" t="s">
-        <v>227</v>
+        <v>269</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E72" s="2" t="s">
-        <v>115</v>
+        <v>216</v>
       </c>
       <c r="F72" s="2"/>
-      <c r="G72" t="s">
-        <v>126</v>
+      <c r="G72" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="H72" s="2"/>
       <c r="I72" s="2"/>
-      <c r="J72" s="2" t="s">
-        <v>22</v>
+      <c r="J72" t="s">
+        <v>16</v>
       </c>
       <c r="K72" s="2"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B73" s="2" t="s">
-        <v>283</v>
+        <v>217</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E73" s="2" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="F73" s="2"/>
-      <c r="G73" s="2" t="s">
-        <v>115</v>
+      <c r="G73" t="s">
+        <v>121</v>
       </c>
       <c r="H73" s="2"/>
       <c r="I73" s="2"/>
-      <c r="J73" s="2"/>
+      <c r="J73" s="2" t="s">
+        <v>21</v>
+      </c>
       <c r="K73" s="2"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B74" s="2" t="s">
-        <v>284</v>
+        <v>270</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" s="6">
         <v>3</v>
       </c>
       <c r="E74" s="2" t="s">
-        <v>231</v>
+        <v>220</v>
       </c>
       <c r="F74" s="2"/>
       <c r="G74" s="2" t="s">
-        <v>230</v>
+        <v>110</v>
       </c>
       <c r="H74" s="2"/>
       <c r="I74" s="2"/>
@@ -2607,20 +2601,19 @@
       <c r="K74" s="2"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A75" s="2"/>
       <c r="B75" s="2" t="s">
-        <v>285</v>
+        <v>271</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" s="6">
         <v>3</v>
       </c>
       <c r="E75" s="2" t="s">
-        <v>50</v>
+        <v>221</v>
       </c>
       <c r="F75" s="2"/>
       <c r="G75" s="2" t="s">
-        <v>38</v>
+        <v>220</v>
       </c>
       <c r="H75" s="2"/>
       <c r="I75" s="2"/>
@@ -2628,19 +2621,20 @@
       <c r="K75" s="2"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A76" s="2"/>
       <c r="B76" s="2" t="s">
-        <v>232</v>
+        <v>272</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" s="6">
         <v>3</v>
       </c>
       <c r="E76" s="2" t="s">
-        <v>233</v>
+        <v>49</v>
       </c>
       <c r="F76" s="2"/>
       <c r="G76" s="2" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="H76" s="2"/>
       <c r="I76" s="2"/>
@@ -2649,17 +2643,18 @@
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B77" s="2" t="s">
-        <v>116</v>
+        <v>222</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E77" s="2" t="s">
-        <v>117</v>
-      </c>
-      <c r="F77" s="2" t="s">
-        <v>130</v>
+        <v>223</v>
+      </c>
+      <c r="F77" s="2"/>
+      <c r="G77" s="2" t="s">
+        <v>49</v>
       </c>
       <c r="H77" s="2"/>
       <c r="I77" s="2"/>
@@ -2668,18 +2663,17 @@
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B78" s="2" t="s">
-        <v>286</v>
+        <v>111</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E78" s="2" t="s">
-        <v>234</v>
-      </c>
-      <c r="F78" s="2"/>
-      <c r="G78" s="2" t="s">
-        <v>117</v>
+        <v>112</v>
+      </c>
+      <c r="F78" s="2" t="s">
+        <v>125</v>
       </c>
       <c r="H78" s="2"/>
       <c r="I78" s="2"/>
@@ -2688,18 +2682,18 @@
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B79" s="2" t="s">
-        <v>287</v>
+        <v>273</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" s="6">
         <v>3</v>
       </c>
       <c r="E79" s="2" t="s">
-        <v>235</v>
+        <v>224</v>
       </c>
       <c r="F79" s="2"/>
       <c r="G79" s="2" t="s">
-        <v>234</v>
+        <v>112</v>
       </c>
       <c r="H79" s="2"/>
       <c r="I79" s="2"/>
@@ -2707,74 +2701,73 @@
       <c r="K79" s="2"/>
     </row>
     <row r="80" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A80" t="s">
-        <v>15</v>
-      </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="2"/>
+      <c r="B80" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="6">
+        <v>3</v>
+      </c>
+      <c r="E80" s="2" t="s">
+        <v>225</v>
+      </c>
       <c r="F80" s="2"/>
-      <c r="G80" s="2"/>
+      <c r="G80" s="2" t="s">
+        <v>224</v>
+      </c>
       <c r="H80" s="2"/>
       <c r="I80" s="2"/>
+      <c r="J80" s="2"/>
+      <c r="K80" s="2"/>
     </row>
     <row r="81" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B81" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>241</v>
+      <c r="A81" t="s">
+        <v>14</v>
       </c>
       <c r="D81" s="6"/>
-      <c r="E81" s="2" t="s">
-        <v>36</v>
-      </c>
+      <c r="E81" s="2"/>
       <c r="F81" s="2"/>
       <c r="G81" s="2"/>
       <c r="H81" s="2"/>
       <c r="I81" s="2"/>
-      <c r="J81" s="2"/>
-      <c r="K81" s="2"/>
     </row>
     <row r="82" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A82" s="2"/>
-      <c r="B82" t="s">
-        <v>118</v>
-      </c>
-      <c r="D82" s="6">
-        <v>3</v>
-      </c>
+      <c r="A82" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C82" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D82" s="6"/>
       <c r="E82" s="2" t="s">
-        <v>119</v>
+        <v>35</v>
       </c>
       <c r="F82" s="2"/>
       <c r="G82" s="2"/>
-      <c r="H82" s="3">
-        <v>44774</v>
-      </c>
+      <c r="H82" s="2"/>
       <c r="I82" s="2"/>
       <c r="J82" s="2"/>
       <c r="K82" s="2"/>
     </row>
     <row r="83" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A83" s="2"/>
-      <c r="B83" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="C83" s="2"/>
+      <c r="B83" t="s">
+        <v>113</v>
+      </c>
       <c r="D83" s="6">
         <v>3</v>
       </c>
       <c r="E83" s="2" t="s">
-        <v>27</v>
+        <v>114</v>
       </c>
       <c r="F83" s="2"/>
-      <c r="G83" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="H83" s="7"/>
+      <c r="G83" s="2"/>
+      <c r="H83" s="3">
+        <v>44774</v>
+      </c>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
       <c r="K83" s="2"/>
@@ -2782,20 +2775,20 @@
     <row r="84" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A84" s="2"/>
       <c r="B84" s="2" t="s">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E84" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F84" s="2"/>
       <c r="G84" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="H84" s="2"/>
+        <v>114</v>
+      </c>
+      <c r="H84" s="7"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2"/>
       <c r="K84" s="2"/>
@@ -2803,18 +2796,18 @@
     <row r="85" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A85" s="2"/>
       <c r="B85" s="2" t="s">
-        <v>64</v>
+        <v>24</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E85" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="F85" s="2"/>
       <c r="G85" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="H85" s="2"/>
       <c r="I85" s="2"/>
@@ -2824,18 +2817,18 @@
     <row r="86" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A86" s="2"/>
       <c r="B86" s="2" t="s">
-        <v>52</v>
+        <v>63</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" s="6">
         <v>3</v>
       </c>
       <c r="E86" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F86" s="2"/>
       <c r="G86" s="2" t="s">
-        <v>53</v>
+        <v>27</v>
       </c>
       <c r="H86" s="2"/>
       <c r="I86" s="2"/>
@@ -2845,18 +2838,18 @@
     <row r="87" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A87" s="2"/>
       <c r="B87" s="2" t="s">
-        <v>186</v>
+        <v>51</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" s="6">
         <v>3</v>
       </c>
       <c r="E87" s="2" t="s">
-        <v>26</v>
+        <v>53</v>
       </c>
       <c r="F87" s="2"/>
       <c r="G87" s="2" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="H87" s="2"/>
       <c r="I87" s="2"/>
@@ -2864,22 +2857,20 @@
       <c r="K87" s="2"/>
     </row>
     <row r="88" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A88" s="2" t="s">
-        <v>15</v>
-      </c>
+      <c r="A88" s="2"/>
       <c r="B88" s="2" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" s="6">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="E88" s="2" t="s">
-        <v>65</v>
+        <v>25</v>
       </c>
       <c r="F88" s="2"/>
       <c r="G88" s="2" t="s">
-        <v>69</v>
+        <v>279</v>
       </c>
       <c r="H88" s="2"/>
       <c r="I88" s="2"/>
@@ -2887,14 +2878,20 @@
       <c r="K88" s="2"/>
     </row>
     <row r="89" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A89" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B89" s="2"/>
+      <c r="A89" s="2"/>
+      <c r="B89" s="2" t="s">
+        <v>172</v>
+      </c>
       <c r="C89" s="2"/>
-      <c r="D89" s="6"/>
-      <c r="E89" s="2"/>
-      <c r="F89" s="2"/>
+      <c r="D89" s="6">
+        <v>9</v>
+      </c>
+      <c r="E89" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F89" s="2" t="s">
+        <v>125</v>
+      </c>
       <c r="G89" s="2"/>
       <c r="H89" s="2"/>
       <c r="I89" s="2"/>
@@ -2903,16 +2900,12 @@
     </row>
     <row r="90" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A90" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90" s="2" t="s">
-        <v>0</v>
-      </c>
+        <v>14</v>
+      </c>
+      <c r="B90" s="2"/>
       <c r="C90" s="2"/>
       <c r="D90" s="6"/>
-      <c r="E90" s="2" t="s">
-        <v>5</v>
-      </c>
+      <c r="E90" s="2"/>
       <c r="F90" s="2"/>
       <c r="G90" s="2"/>
       <c r="H90" s="2"/>
@@ -2921,76 +2914,74 @@
       <c r="K90" s="2"/>
     </row>
     <row r="91" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A91" s="2"/>
+      <c r="A91" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="B91" s="2" t="s">
-        <v>120</v>
+        <v>0</v>
       </c>
       <c r="C91" s="2"/>
-      <c r="D91" s="6">
-        <v>3</v>
-      </c>
+      <c r="D91" s="6"/>
       <c r="E91" s="2" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="F91" s="2"/>
-      <c r="G91" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H91" s="7"/>
+      <c r="G91" s="2"/>
+      <c r="H91" s="2"/>
       <c r="I91" s="2"/>
       <c r="J91" s="2"/>
       <c r="K91" s="2"/>
     </row>
     <row r="92" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B92" t="s">
-        <v>173</v>
-      </c>
-      <c r="D92" s="5">
+      <c r="A92" s="2"/>
+      <c r="B92" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C92" s="2"/>
+      <c r="D92" s="6">
         <v>3</v>
       </c>
       <c r="E92" s="2" t="s">
-        <v>255</v>
-      </c>
+        <v>33</v>
+      </c>
+      <c r="F92" s="2"/>
       <c r="G92" s="2" t="s">
-        <v>34</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="H92" s="7"/>
+      <c r="I92" s="2"/>
+      <c r="J92" s="2"/>
+      <c r="K92" s="2"/>
     </row>
     <row r="93" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A93" s="2"/>
-      <c r="B93" s="2" t="s">
+      <c r="B93" t="s">
+        <v>284</v>
+      </c>
+      <c r="D93" s="5">
+        <v>3</v>
+      </c>
+      <c r="E93" s="2" t="s">
         <v>244</v>
       </c>
-      <c r="C93" s="2"/>
-      <c r="D93" s="6">
-        <v>3</v>
-      </c>
-      <c r="E93" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="F93" s="2"/>
       <c r="G93" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="H93" s="2"/>
-      <c r="I93" s="2"/>
-      <c r="J93" s="2"/>
-      <c r="K93" s="2"/>
+        <v>33</v>
+      </c>
     </row>
     <row r="94" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A94" s="2"/>
       <c r="B94" s="2" t="s">
-        <v>179</v>
+        <v>234</v>
       </c>
       <c r="C94" s="2"/>
       <c r="D94" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E94" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="F94" s="2"/>
       <c r="G94" s="2" t="s">
-        <v>35</v>
+        <v>244</v>
       </c>
       <c r="H94" s="2"/>
       <c r="I94" s="2"/>
@@ -3000,18 +2991,18 @@
     <row r="95" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A95" s="2"/>
       <c r="B95" s="2" t="s">
-        <v>121</v>
+        <v>171</v>
       </c>
       <c r="C95" s="2"/>
       <c r="D95" s="6">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E95" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="F95" s="2"/>
       <c r="G95" s="2" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H95" s="2"/>
       <c r="I95" s="2"/>
@@ -3021,18 +3012,18 @@
     <row r="96" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A96" s="2"/>
       <c r="B96" s="2" t="s">
-        <v>245</v>
+        <v>116</v>
       </c>
       <c r="C96" s="2"/>
       <c r="D96" s="6">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E96" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="F96" s="2"/>
       <c r="G96" s="2" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="H96" s="2"/>
       <c r="I96" s="2"/>
@@ -3042,18 +3033,18 @@
     <row r="97" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A97" s="2"/>
       <c r="B97" s="2" t="s">
-        <v>178</v>
+        <v>235</v>
       </c>
       <c r="C97" s="2"/>
       <c r="D97" s="6">
         <v>3</v>
       </c>
       <c r="E97" s="2" t="s">
-        <v>71</v>
+        <v>31</v>
       </c>
       <c r="F97" s="2"/>
       <c r="G97" s="2" t="s">
-        <v>32</v>
+        <v>42</v>
       </c>
       <c r="H97" s="2"/>
       <c r="I97" s="2"/>
@@ -3063,18 +3054,18 @@
     <row r="98" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A98" s="2"/>
       <c r="B98" s="2" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C98" s="2"/>
       <c r="D98" s="6">
         <v>3</v>
       </c>
       <c r="E98" s="2" t="s">
-        <v>21</v>
+        <v>68</v>
       </c>
       <c r="F98" s="2"/>
       <c r="G98" s="2" t="s">
-        <v>185</v>
+        <v>31</v>
       </c>
       <c r="H98" s="2"/>
       <c r="I98" s="2"/>
@@ -3084,18 +3075,18 @@
     <row r="99" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A99" s="2"/>
       <c r="B99" s="2" t="s">
-        <v>122</v>
+        <v>278</v>
       </c>
       <c r="C99" s="2"/>
       <c r="D99" s="6">
         <v>3</v>
       </c>
       <c r="E99" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="F99" s="2"/>
       <c r="G99" s="2" t="s">
-        <v>21</v>
+        <v>176</v>
       </c>
       <c r="H99" s="2"/>
       <c r="I99" s="2"/>
@@ -3105,18 +3096,18 @@
     <row r="100" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A100" s="2"/>
       <c r="B100" s="2" t="s">
-        <v>103</v>
+        <v>117</v>
       </c>
       <c r="C100" s="2"/>
       <c r="D100" s="6">
         <v>3</v>
       </c>
       <c r="E100" s="2" t="s">
-        <v>67</v>
+        <v>32</v>
       </c>
       <c r="F100" s="2"/>
       <c r="G100" s="2" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
       <c r="H100" s="2"/>
       <c r="I100" s="2"/>
@@ -3126,17 +3117,18 @@
     <row r="101" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A101" s="2"/>
       <c r="B101" s="2" t="s">
-        <v>97</v>
+        <v>277</v>
       </c>
       <c r="C101" s="2"/>
       <c r="D101" s="6">
         <v>3</v>
       </c>
       <c r="E101" s="2" t="s">
-        <v>68</v>
-      </c>
+        <v>279</v>
+      </c>
+      <c r="F101" s="2"/>
       <c r="G101" s="2" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="H101" s="2"/>
       <c r="I101" s="2"/>
@@ -3146,18 +3138,17 @@
     <row r="102" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A102" s="2"/>
       <c r="B102" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C102" s="2"/>
       <c r="D102" s="6">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="E102" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F102" s="2"/>
+        <v>66</v>
+      </c>
       <c r="G102" s="2" t="s">
-        <v>68</v>
+        <v>25</v>
       </c>
       <c r="H102" s="2"/>
       <c r="I102" s="2"/>
@@ -3167,18 +3158,18 @@
     <row r="103" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A103" s="2"/>
       <c r="B103" s="2" t="s">
-        <v>249</v>
+        <v>93</v>
       </c>
       <c r="C103" s="2"/>
       <c r="D103" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E103" s="2" t="s">
-        <v>148</v>
+        <v>67</v>
       </c>
       <c r="F103" s="2"/>
       <c r="G103" s="2" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H103" s="2"/>
       <c r="I103" s="2"/>
@@ -3188,18 +3179,18 @@
     <row r="104" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A104" s="2"/>
       <c r="B104" s="2" t="s">
-        <v>95</v>
+        <v>239</v>
       </c>
       <c r="C104" s="2"/>
       <c r="D104" s="6">
         <v>3</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="F104" s="2"/>
       <c r="G104" s="2" t="s">
-        <v>112</v>
+        <v>64</v>
       </c>
       <c r="H104" s="2"/>
       <c r="I104" s="2"/>
@@ -3209,7 +3200,7 @@
     <row r="105" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A105" s="2"/>
       <c r="B105" s="2" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="C105" s="2"/>
       <c r="D105" s="6">
@@ -3220,7 +3211,7 @@
       </c>
       <c r="F105" s="2"/>
       <c r="G105" s="2" t="s">
-        <v>72</v>
+        <v>143</v>
       </c>
       <c r="H105" s="2"/>
       <c r="I105" s="2"/>
@@ -3229,7 +3220,7 @@
     </row>
     <row r="106" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A106" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B106" s="2"/>
       <c r="C106" s="2"/>
@@ -3244,7 +3235,7 @@
     </row>
     <row r="107" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A107" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>0</v>
@@ -3258,29 +3249,29 @@
       <c r="H107" s="2"/>
       <c r="I107" s="2"/>
       <c r="J107" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="108" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A108" s="2"/>
       <c r="B108" s="2" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C108" s="2"/>
       <c r="D108" s="6">
         <v>0</v>
       </c>
       <c r="E108" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="F108" s="2"/>
       <c r="G108" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="H108" s="2"/>
       <c r="I108" s="2"/>
       <c r="J108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="109" spans="1:11" x14ac:dyDescent="0.35">
@@ -3290,32 +3281,32 @@
       </c>
       <c r="C109" s="2"/>
       <c r="D109" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E109" s="2" t="s">
         <v>10</v>
       </c>
       <c r="F109" s="2"/>
       <c r="G109" s="2" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="H109" s="2"/>
       <c r="I109" s="2"/>
       <c r="J109" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="110" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A110" s="2"/>
       <c r="B110" s="2" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C110" s="2"/>
       <c r="D110" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E110" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F110" s="2"/>
       <c r="G110" s="2" t="s">
@@ -3324,87 +3315,87 @@
       <c r="H110" s="2"/>
       <c r="I110" s="2"/>
       <c r="J110" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="111" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A111" s="2"/>
       <c r="B111" s="2" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C111" s="2"/>
       <c r="D111" s="6">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="E111" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F111" s="2"/>
       <c r="G111" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H111" s="2"/>
       <c r="I111" s="2"/>
       <c r="J111" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="112" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A112" s="2"/>
       <c r="B112" s="2" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C112" s="2"/>
       <c r="D112" s="6">
         <v>6</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="F112" s="2"/>
       <c r="G112" s="2" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="H112" s="2"/>
       <c r="I112" s="2"/>
       <c r="J112" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="113" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A113" s="2"/>
       <c r="B113" s="2" t="s">
-        <v>273</v>
+        <v>281</v>
       </c>
       <c r="C113" s="2"/>
       <c r="D113" s="6">
         <v>3</v>
       </c>
       <c r="E113" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="F113" s="2"/>
-      <c r="G113" s="2" t="s">
-        <v>111</v>
-      </c>
+        <v>142</v>
+      </c>
+      <c r="F113" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G113" s="2"/>
       <c r="H113" s="2"/>
       <c r="I113" s="2"/>
     </row>
     <row r="114" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A114" s="2"/>
       <c r="B114" s="2" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C114" s="2"/>
       <c r="D114" s="6">
         <v>3</v>
       </c>
       <c r="E114" s="2" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="F114" s="2"/>
       <c r="G114" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="H114" s="2"/>
       <c r="I114" s="2"/>
@@ -3412,37 +3403,37 @@
     <row r="115" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A115" s="2"/>
       <c r="B115" s="2" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C115" s="2"/>
       <c r="D115" s="6">
         <v>0</v>
       </c>
       <c r="E115" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F115" s="2"/>
-      <c r="G115" s="2" t="s">
-        <v>148</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="F115" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="G115" s="2"/>
       <c r="H115" s="2"/>
       <c r="I115" s="2"/>
     </row>
     <row r="116" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A116" s="2"/>
       <c r="B116" s="2" t="s">
-        <v>250</v>
+        <v>280</v>
       </c>
       <c r="C116" s="2"/>
       <c r="D116" s="6">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E116" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="F116" s="2"/>
       <c r="G116" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="H116" s="2"/>
       <c r="I116" s="2"/>
@@ -3450,18 +3441,18 @@
     <row r="117" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A117" s="2"/>
       <c r="B117" s="2" t="s">
-        <v>251</v>
+        <v>240</v>
       </c>
       <c r="C117" s="2"/>
       <c r="D117" s="6">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E117" s="2" t="s">
-        <v>252</v>
+        <v>241</v>
       </c>
       <c r="F117" s="2"/>
       <c r="G117" s="2" t="s">
-        <v>253</v>
+        <v>242</v>
       </c>
       <c r="H117" s="2"/>
       <c r="I117" s="2"/>
@@ -3469,27 +3460,27 @@
     <row r="118" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A118" s="2"/>
       <c r="B118" s="2" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
       <c r="C118" s="2"/>
       <c r="D118" s="6">
         <v>3</v>
       </c>
       <c r="E118" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="G118" t="s">
-        <v>125</v>
+        <v>107</v>
+      </c>
+      <c r="G118" s="2" t="s">
+        <v>69</v>
       </c>
       <c r="H118" s="2"/>
       <c r="I118" s="2"/>
       <c r="J118" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="119" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A119" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B119" s="2"/>
       <c r="C119" s="2"/>
@@ -3504,17 +3495,17 @@
     </row>
     <row r="120" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
-        <v>220</v>
+        <v>210</v>
       </c>
       <c r="B120" t="s">
         <v>0</v>
       </c>
       <c r="C120" s="2" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="D120" s="6"/>
       <c r="E120" s="2" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="F120" s="2"/>
       <c r="G120" s="2"/>
@@ -3524,18 +3515,18 @@
     <row r="121" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A121" s="2"/>
       <c r="B121" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C121" s="2"/>
       <c r="D121" s="6">
         <v>6</v>
       </c>
       <c r="E121" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F121" s="2"/>
       <c r="G121" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="H121" s="2"/>
       <c r="I121" s="2"/>
@@ -3544,68 +3535,62 @@
     </row>
     <row r="122" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
-        <v>254</v>
+        <v>243</v>
       </c>
       <c r="D122" s="5">
         <v>6</v>
       </c>
       <c r="E122" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="G122" s="2" t="s">
-        <v>256</v>
+        <v>245</v>
       </c>
     </row>
     <row r="123" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D123" s="5">
         <v>0</v>
       </c>
       <c r="E123" s="2" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="G123" s="2" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C124" s="2"/>
-      <c r="D124" s="6">
-        <v>6</v>
+      <c r="B124" t="s">
+        <v>285</v>
+      </c>
+      <c r="D124" s="5">
+        <v>3</v>
       </c>
       <c r="E124" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="F124" s="2"/>
-      <c r="G124" t="s">
-        <v>170</v>
-      </c>
-      <c r="H124" s="2"/>
-      <c r="I124" s="2"/>
-      <c r="J124" s="2"/>
-      <c r="K124" s="2"/>
+        <v>286</v>
+      </c>
+      <c r="F124" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="G124" s="2"/>
     </row>
     <row r="125" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A125" s="2"/>
       <c r="B125" s="2" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="C125" s="2"/>
       <c r="D125" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E125" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F125" s="2"/>
-      <c r="G125" s="2" t="s">
-        <v>46</v>
+      <c r="G125" t="s">
+        <v>164</v>
       </c>
       <c r="H125" s="2"/>
       <c r="I125" s="2"/>
@@ -3615,18 +3600,18 @@
     <row r="126" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A126" s="2"/>
       <c r="B126" s="2" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C126" s="2"/>
       <c r="D126" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E126" s="2" t="s">
-        <v>92</v>
+        <v>46</v>
       </c>
       <c r="F126" s="2"/>
       <c r="G126" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="H126" s="2"/>
       <c r="I126" s="2"/>
@@ -3634,49 +3619,51 @@
       <c r="K126" s="2"/>
     </row>
     <row r="127" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A127" t="s">
-        <v>15</v>
-      </c>
-      <c r="D127" s="6"/>
-      <c r="E127" s="2"/>
+      <c r="A127" s="2"/>
+      <c r="B127" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C127" s="2"/>
+      <c r="D127" s="6">
+        <v>0</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>89</v>
+      </c>
       <c r="F127" s="2"/>
-      <c r="G127" s="2"/>
+      <c r="G127" s="2" t="s">
+        <v>46</v>
+      </c>
       <c r="H127" s="2"/>
       <c r="I127" s="2"/>
+      <c r="J127" s="2"/>
+      <c r="K127" s="2"/>
     </row>
     <row r="128" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A128" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="B128" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C128" s="2"/>
+      <c r="A128" t="s">
+        <v>14</v>
+      </c>
       <c r="D128" s="6"/>
-      <c r="E128" s="2" t="s">
-        <v>222</v>
-      </c>
+      <c r="E128" s="2"/>
       <c r="F128" s="2"/>
       <c r="G128" s="2"/>
       <c r="H128" s="2"/>
       <c r="I128" s="2"/>
-      <c r="J128" s="2"/>
-      <c r="K128" s="2"/>
     </row>
     <row r="129" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B129" t="s">
-        <v>261</v>
-      </c>
-      <c r="D129" s="6">
-        <v>7</v>
-      </c>
+      <c r="A129" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B129" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C129" s="2"/>
+      <c r="D129" s="6"/>
       <c r="E129" s="2" t="s">
-        <v>263</v>
+        <v>212</v>
       </c>
       <c r="F129" s="2"/>
-      <c r="G129" s="2" t="s">
-        <v>45</v>
-      </c>
+      <c r="G129" s="2"/>
       <c r="H129" s="2"/>
       <c r="I129" s="2"/>
       <c r="J129" s="2"/>
@@ -3684,17 +3671,17 @@
     </row>
     <row r="130" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B130" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="D130" s="6">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E130" s="2" t="s">
-        <v>264</v>
+        <v>252</v>
       </c>
       <c r="F130" s="2"/>
       <c r="G130" s="2" t="s">
-        <v>169</v>
+        <v>44</v>
       </c>
       <c r="H130" s="2"/>
       <c r="I130" s="2"/>
@@ -3703,324 +3690,360 @@
     </row>
     <row r="131" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B131" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="D131" s="6">
         <v>9</v>
       </c>
       <c r="E131" s="2" t="s">
-        <v>74</v>
+        <v>253</v>
       </c>
       <c r="F131" s="2"/>
       <c r="G131" s="2" t="s">
-        <v>265</v>
+        <v>163</v>
       </c>
       <c r="H131" s="2"/>
       <c r="I131" s="2"/>
+      <c r="J131" s="2"/>
+      <c r="K131" s="2"/>
     </row>
     <row r="132" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B132" t="s">
-        <v>288</v>
+        <v>246</v>
       </c>
       <c r="D132" s="6">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E132" s="2" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="F132" s="2"/>
       <c r="G132" s="2" t="s">
-        <v>74</v>
+        <v>254</v>
       </c>
       <c r="H132" s="2"/>
       <c r="I132" s="2"/>
     </row>
     <row r="133" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B133" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="D133" s="6">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="E133" s="2" t="s">
-        <v>267</v>
+        <v>72</v>
       </c>
       <c r="F133" s="2"/>
       <c r="G133" s="2" t="s">
-        <v>124</v>
+        <v>71</v>
       </c>
       <c r="H133" s="2"/>
       <c r="I133" s="2"/>
     </row>
     <row r="134" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B134" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
       <c r="D134" s="6">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E134" s="2" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F134" s="2"/>
-      <c r="G134" t="s">
-        <v>269</v>
+      <c r="G134" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="H134" s="2"/>
       <c r="I134" s="2"/>
     </row>
     <row r="135" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B135" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="D135" s="6">
         <v>3</v>
       </c>
       <c r="E135" s="2" t="s">
-        <v>39</v>
+        <v>249</v>
       </c>
       <c r="F135" s="2"/>
-      <c r="G135" s="2" t="s">
-        <v>260</v>
+      <c r="G135" t="s">
+        <v>258</v>
       </c>
       <c r="H135" s="2"/>
       <c r="I135" s="2"/>
     </row>
     <row r="136" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B136" t="s">
-        <v>268</v>
+        <v>248</v>
       </c>
       <c r="D136" s="6">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E136" s="2" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="F136" s="2"/>
       <c r="G136" s="2" t="s">
-        <v>39</v>
+        <v>249</v>
       </c>
       <c r="H136" s="2"/>
       <c r="I136" s="2"/>
     </row>
     <row r="137" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B137" t="s">
-        <v>270</v>
+        <v>257</v>
       </c>
       <c r="D137" s="6">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="E137" s="2" t="s">
-        <v>271</v>
+        <v>73</v>
       </c>
       <c r="F137" s="2"/>
       <c r="G137" s="2" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="H137" s="2"/>
       <c r="I137" s="2"/>
     </row>
     <row r="138" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A138" t="s">
-        <v>15</v>
-      </c>
+      <c r="B138" t="s">
+        <v>259</v>
+      </c>
+      <c r="D138" s="6">
+        <v>6</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="F138" s="2"/>
+      <c r="G138" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H138" s="2"/>
+      <c r="I138" s="2"/>
     </row>
     <row r="139" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A139" t="s">
-        <v>59</v>
-      </c>
       <c r="B139" t="s">
+        <v>288</v>
+      </c>
+      <c r="D139" s="6">
+        <v>12</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>289</v>
+      </c>
+      <c r="F139" s="2"/>
+      <c r="G139" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="H139" s="2"/>
+      <c r="I139" s="2"/>
+    </row>
+    <row r="140" spans="1:11" ht="13.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A140" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A141" t="s">
+        <v>58</v>
+      </c>
+      <c r="B141" t="s">
         <v>0</v>
       </c>
-      <c r="C139" t="s">
-        <v>243</v>
-      </c>
-      <c r="E139" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B140" t="s">
-        <v>149</v>
-      </c>
-      <c r="D140" s="5">
-        <v>9</v>
-      </c>
-      <c r="E140" t="s">
-        <v>79</v>
-      </c>
-      <c r="G140" s="2" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="B141" t="s">
-        <v>77</v>
-      </c>
-      <c r="D141" s="5">
-        <v>3</v>
+      <c r="C141" t="s">
+        <v>233</v>
       </c>
       <c r="E141" t="s">
-        <v>80</v>
-      </c>
-      <c r="G141" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="142" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B142" t="s">
-        <v>56</v>
+        <v>144</v>
       </c>
       <c r="D142" s="5">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="E142" t="s">
-        <v>82</v>
-      </c>
-      <c r="G142" t="s">
-        <v>80</v>
+        <v>76</v>
+      </c>
+      <c r="G142" s="2" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="143" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B143" t="s">
-        <v>105</v>
+        <v>74</v>
       </c>
       <c r="D143" s="5">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E143" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
       <c r="G143" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
     </row>
     <row r="144" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B144" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="D144" s="5">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="E144" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="G144" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="145" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B145" t="s">
-        <v>62</v>
+        <v>100</v>
       </c>
       <c r="D145" s="5">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E145" t="s">
-        <v>83</v>
-      </c>
-      <c r="G145" s="2" t="s">
-        <v>272</v>
+        <v>86</v>
+      </c>
+      <c r="G145" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="146" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B146" t="s">
-        <v>98</v>
+        <v>59</v>
       </c>
       <c r="D146" s="5">
         <v>4</v>
       </c>
       <c r="E146" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
       <c r="G146" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="147" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B147" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="D147" s="5">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="E147" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="G147" s="2" t="s">
-        <v>84</v>
+        <v>256</v>
       </c>
     </row>
     <row r="148" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B148" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="D148" s="5">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="E148" t="s">
-        <v>86</v>
-      </c>
-      <c r="G148" s="2" t="s">
-        <v>114</v>
+        <v>81</v>
+      </c>
+      <c r="G148" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="149" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B149" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D149" s="5">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E149" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="G149" s="2" t="s">
-        <v>271</v>
+        <v>81</v>
       </c>
     </row>
     <row r="150" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B150" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="D150" s="5">
         <v>6</v>
       </c>
       <c r="E150" t="s">
-        <v>151</v>
-      </c>
-      <c r="G150" t="s">
-        <v>87</v>
+        <v>83</v>
+      </c>
+      <c r="G150" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="151" spans="1:11" x14ac:dyDescent="0.35">
       <c r="B151" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D151" s="5">
         <v>9</v>
       </c>
       <c r="E151" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G151" s="2" t="s">
-        <v>151</v>
+        <v>260</v>
       </c>
     </row>
     <row r="152" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A152" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-      <c r="D152" s="6"/>
-      <c r="E152" s="2"/>
-      <c r="F152" s="2"/>
-      <c r="G152" s="2"/>
-      <c r="H152" s="2"/>
-      <c r="I152" s="2"/>
-      <c r="J152" s="2"/>
-      <c r="K152" s="2"/>
+      <c r="B152" t="s">
+        <v>145</v>
+      </c>
+      <c r="D152" s="5">
+        <v>6</v>
+      </c>
+      <c r="E152" t="s">
+        <v>146</v>
+      </c>
+      <c r="G152" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="B153" t="s">
+        <v>56</v>
+      </c>
+      <c r="D153" s="5">
+        <v>9</v>
+      </c>
+      <c r="E153" t="s">
+        <v>85</v>
+      </c>
+      <c r="G153" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="A154" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B154" s="2"/>
+      <c r="C154" s="2"/>
+      <c r="D154" s="6"/>
+      <c r="E154" s="2"/>
+      <c r="F154" s="2"/>
+      <c r="G154" s="2"/>
+      <c r="H154" s="2"/>
+      <c r="I154" s="2"/>
+      <c r="J154" s="2"/>
+      <c r="K154" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>